<commit_message>
Added tags page and logic.
</commit_message>
<xml_diff>
--- a/docs/JNLTrav.xlsx
+++ b/docs/JNLTrav.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po01imj\Documents\GitHub\P_AppMobile-Passion-Lecture\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ADB0AA-DFA5-4EFA-8429-E26A1BC47E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F9BFED-5F92-4DC8-8650-2DA0502B99F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -149,6 +149,18 @@
   </si>
   <si>
     <t>Développement du page library</t>
+  </si>
+  <si>
+    <t>Développement du page library (lien au settings, style, etc)</t>
+  </si>
+  <si>
+    <t>Développement du page library ( les tags, style)</t>
+  </si>
+  <si>
+    <t>Développement du tags (logic)</t>
+  </si>
+  <si>
+    <t>Research sur creation dynamic de elements via c#</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1078,10 @@
                 <c:formatCode>hh\ "h"\ mm\ "min"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>3.8194444444444448E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18055555555555555</c:v>
+                  <c:v>0.2951388888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2000,7 +2012,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2053,7 +2065,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 8 heurs 0 minutes</v>
+        <v>0 jours 11 heurs 10 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2072,11 +2084,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>240</v>
+        <v>430</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>480</v>
+        <v>670</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2340,15 +2352,23 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="str">
+      <c r="A15" s="17">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="51"/>
+        <v>17</v>
+      </c>
+      <c r="B15" s="51">
+        <v>45404</v>
+      </c>
       <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="37"/>
+      <c r="D15" s="53">
+        <v>50</v>
+      </c>
+      <c r="E15" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>36</v>
+      </c>
       <c r="G15" s="18"/>
       <c r="M15" t="s">
         <v>22</v>
@@ -2361,60 +2381,92 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="47"/>
+        <v>17</v>
+      </c>
+      <c r="B16" s="47">
+        <v>45404</v>
+      </c>
       <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="37"/>
+      <c r="D16" s="49">
+        <v>40</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>37</v>
+      </c>
       <c r="G16" s="16"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="str">
+      <c r="A17" s="17">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="51"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="51">
+        <v>45404</v>
+      </c>
       <c r="C17" s="52"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="37"/>
+      <c r="D17" s="53">
+        <v>30</v>
+      </c>
+      <c r="E17" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>38</v>
+      </c>
       <c r="G17" s="18"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="47"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="47">
+        <v>45404</v>
+      </c>
       <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="37"/>
+      <c r="D18" s="49">
+        <v>25</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>39</v>
+      </c>
       <c r="G18" s="16"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="str">
+      <c r="A19" s="17">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="51"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="51">
+        <v>45404</v>
+      </c>
       <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="37"/>
+      <c r="D19" s="53">
+        <v>45</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>38</v>
+      </c>
       <c r="G19" s="18"/>
       <c r="O19">
         <v>55</v>
@@ -8665,7 +8717,7 @@
       </c>
       <c r="B4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C4" s="26" t="str">
         <f>'Journal de travail'!M8</f>
@@ -8673,7 +8725,7 @@
       </c>
       <c r="D4" s="34">
         <f>(A4+B4)/1440</f>
-        <v>2.0833333333333332E-2</v>
+        <v>3.8194444444444448E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -8683,7 +8735,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>140</v>
+        <v>305</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8691,7 +8743,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.18055555555555555</v>
+        <v>0.2951388888888889</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8800,7 +8852,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.24999999999999997</v>
+        <v>0.38194444444444453</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9037,15 +9089,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9054,6 +9097,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9076,14 +9128,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9092,4 +9136,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>